<commit_message>
Added credit card documents
</commit_message>
<xml_diff>
--- a/Wedding/Vendor Costings.xlsx
+++ b/Wedding/Vendor Costings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenny.Lim\Desktop\Lighthouse Repos\About\Wedding\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FABFAE57-67C9-418E-843D-9786B8E25B5F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400B62F1-FA5A-467C-95C3-26378FA8AF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="23500" xr2:uid="{32757893-5A81-40E6-85E9-2923B5788D18}"/>
   </bookViews>
@@ -599,7 +599,7 @@
   <dimension ref="A1:N102"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>